<commit_message>
solucion de error con profesores
- Se arregla el error cuando existen multiples profesores
- Se quitan los segundos de la hora
- Se agrega el archivo final generado
</commit_message>
<xml_diff>
--- a/web/MyExcel.xlsx
+++ b/web/MyExcel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="356">
   <si>
     <t>Asignatura</t>
   </si>
@@ -92,13 +92,13 @@
     <t>CC1</t>
   </si>
   <si>
-    <t>10:30:00 - 11:30:00</t>
+    <t>10:30 - 11:30</t>
   </si>
   <si>
     <t>C8</t>
   </si>
   <si>
-    <t>08:30:00 - 09:30:00</t>
+    <t>08:30 - 09:30</t>
   </si>
   <si>
     <t>Acomp: Álgebra Superior</t>
@@ -125,7 +125,7 @@
     <t>Chan García</t>
   </si>
   <si>
-    <t>07:00:00 - 08:30:00</t>
+    <t>07:00 - 08:30</t>
   </si>
   <si>
     <t>Acomp: Investigación de Operaciones</t>
@@ -170,7 +170,7 @@
     <t>CC3</t>
   </si>
   <si>
-    <t>07:00:00 - 08:00:00</t>
+    <t>07:00 - 08:00</t>
   </si>
   <si>
     <t>Acomp: Procesos Estocásticos</t>
@@ -518,7 +518,7 @@
     <t xml:space="preserve">Carlos/Ricardo </t>
   </si>
   <si>
-    <t>Carlos/Legarda Sáenz</t>
+    <t>Brito Loeza/Legarda Sáenz</t>
   </si>
   <si>
     <t>Control II</t>
@@ -557,7 +557,7 @@
     <t>Eddie/Jorge Ricardo</t>
   </si>
   <si>
-    <t>Eddie/Gómez Montalvo</t>
+    <t>Aparicio Landa/Gómez Montalvo</t>
   </si>
   <si>
     <t>Desarrollo Curricular</t>
@@ -593,7 +593,7 @@
     <t>Carlos Benito/Edwin Jesús</t>
   </si>
   <si>
-    <t>Carlos Benito/León Bojórquez</t>
+    <t>Mojica Ruíz/León Bojórquez</t>
   </si>
   <si>
     <t>Didáctica de la Geometría</t>
@@ -650,7 +650,7 @@
     <t>C2</t>
   </si>
   <si>
-    <t>07:00:00 - 09:00:00</t>
+    <t>07:00 - 09:00</t>
   </si>
   <si>
     <t>Ecuaciones Diferenciales I</t>
@@ -680,10 +680,10 @@
     <t>C1</t>
   </si>
   <si>
-    <t>08:00:00 - 09:30:00</t>
-  </si>
-  <si>
-    <t>08:30:00 - 10:00:00</t>
+    <t>08:00 - 09:30</t>
+  </si>
+  <si>
+    <t>08:30 - 10:00</t>
   </si>
   <si>
     <t>C6</t>
@@ -933,6 +933,12 @@
   </si>
   <si>
     <t>Probabilidad II</t>
+  </si>
+  <si>
+    <t>Aarón Abraham/Raúl Antonio/Antonio Armando/Anabel</t>
+  </si>
+  <si>
+    <t>Aguayo González/Aguilar Vera/Aguileta Güemez/Martín González</t>
   </si>
   <si>
     <t>Procesos Estocásticos</t>
@@ -1162,7 +1168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -1183,6 +1189,9 @@
     </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="4" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1483,13 +1492,13 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:V149"/>
+  <dimension ref="A1:V148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="21" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="V149" sqref="V149"/>
+      <selection pane="bottomRight" activeCell="A148" sqref="A148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1497,23 +1506,23 @@
     <col min="1" max="1" width="69.840088" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="26.707764" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="10.140381" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="26.707764" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="29.707031" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="51.273193" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="62.698975" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="8.140869" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="7.141113" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="9.140625" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="10.140381" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="9.140625" bestFit="true" customWidth="true" style="0"/>
     <col min="11" max="11" width="6.141357" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="20.423584" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="14.282227" bestFit="true" customWidth="true" style="0"/>
     <col min="13" max="13" width="6.141357" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="20.423584" bestFit="true" customWidth="true" style="0"/>
+    <col min="14" max="14" width="14.282227" bestFit="true" customWidth="true" style="0"/>
     <col min="15" max="15" width="6.141357" bestFit="true" customWidth="true" style="0"/>
-    <col min="16" max="16" width="20.423584" bestFit="true" customWidth="true" style="0"/>
+    <col min="16" max="16" width="14.282227" bestFit="true" customWidth="true" style="0"/>
     <col min="17" max="17" width="6.141357" bestFit="true" customWidth="true" style="0"/>
-    <col min="18" max="18" width="20.423584" bestFit="true" customWidth="true" style="0"/>
+    <col min="18" max="18" width="14.282227" bestFit="true" customWidth="true" style="0"/>
     <col min="19" max="19" width="6.141357" bestFit="true" customWidth="true" style="0"/>
-    <col min="20" max="20" width="20.423584" bestFit="true" customWidth="true" style="0"/>
+    <col min="20" max="20" width="14.282227" bestFit="true" customWidth="true" style="0"/>
     <col min="21" max="21" width="6.141357" bestFit="true" customWidth="true" style="0"/>
     <col min="22" max="22" width="8.140869" bestFit="true" customWidth="true" style="0"/>
   </cols>
@@ -1623,7 +1632,7 @@
       </c>
     </row>
     <row r="3" spans="1:22">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1667,7 +1676,7 @@
       <c r="V3" s="6"/>
     </row>
     <row r="4" spans="1:22">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1703,7 +1712,7 @@
       <c r="V4" s="6"/>
     </row>
     <row r="5" spans="1:22">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1743,7 +1752,7 @@
       <c r="V5" s="6"/>
     </row>
     <row r="6" spans="1:22">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="7" t="s">
         <v>37</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1779,7 +1788,7 @@
       <c r="V6" s="6"/>
     </row>
     <row r="7" spans="1:22">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="7" t="s">
         <v>40</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1815,7 +1824,7 @@
       <c r="V7" s="6"/>
     </row>
     <row r="8" spans="1:22">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1851,7 +1860,7 @@
       <c r="V8" s="6"/>
     </row>
     <row r="9" spans="1:22">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="7" t="s">
         <v>46</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1887,7 +1896,7 @@
       <c r="V9" s="6"/>
     </row>
     <row r="10" spans="1:22">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="7" t="s">
         <v>47</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1927,7 +1936,7 @@
       <c r="V10" s="6"/>
     </row>
     <row r="11" spans="1:22">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="7" t="s">
         <v>52</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1963,7 +1972,7 @@
       <c r="V11" s="6"/>
     </row>
     <row r="12" spans="1:22">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="7" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1999,7 +2008,7 @@
       <c r="V12" s="6"/>
     </row>
     <row r="13" spans="1:22">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="7" t="s">
         <v>56</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -2035,7 +2044,7 @@
       <c r="V13" s="6"/>
     </row>
     <row r="14" spans="1:22">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="7" t="s">
         <v>57</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -2075,7 +2084,7 @@
       <c r="V14" s="6"/>
     </row>
     <row r="15" spans="1:22">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="7" t="s">
         <v>62</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -2119,7 +2128,7 @@
       <c r="V15" s="6"/>
     </row>
     <row r="16" spans="1:22">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="7" t="s">
         <v>67</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -2159,7 +2168,7 @@
       <c r="V16" s="6"/>
     </row>
     <row r="17" spans="1:22">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="7" t="s">
         <v>72</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -2205,7 +2214,7 @@
       <c r="V17" s="6"/>
     </row>
     <row r="18" spans="1:22">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="7" t="s">
         <v>76</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -2245,7 +2254,7 @@
       <c r="V18" s="6"/>
     </row>
     <row r="19" spans="1:22">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="7" t="s">
         <v>76</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -2285,7 +2294,7 @@
       <c r="V19" s="6"/>
     </row>
     <row r="20" spans="1:22">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="7" t="s">
         <v>82</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -2327,7 +2336,7 @@
       <c r="V20" s="6"/>
     </row>
     <row r="21" spans="1:22">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="7" t="s">
         <v>85</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -2367,7 +2376,7 @@
       <c r="V21" s="6"/>
     </row>
     <row r="22" spans="1:22">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="7" t="s">
         <v>86</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -2407,7 +2416,7 @@
       <c r="V22" s="6"/>
     </row>
     <row r="23" spans="1:22">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="7" t="s">
         <v>88</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -2449,7 +2458,7 @@
       <c r="V23" s="6"/>
     </row>
     <row r="24" spans="1:22">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="7" t="s">
         <v>92</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -2491,7 +2500,7 @@
       <c r="V24" s="6"/>
     </row>
     <row r="25" spans="1:22">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="7" t="s">
         <v>93</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -2531,7 +2540,7 @@
       <c r="V25" s="6"/>
     </row>
     <row r="26" spans="1:22">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="7" t="s">
         <v>96</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -2571,7 +2580,7 @@
       <c r="V26" s="6"/>
     </row>
     <row r="27" spans="1:22">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="7" t="s">
         <v>96</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -2613,7 +2622,7 @@
       <c r="V27" s="6"/>
     </row>
     <row r="28" spans="1:22">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="7" t="s">
         <v>101</v>
       </c>
       <c r="B28" s="3" t="s">
@@ -2653,7 +2662,7 @@
       <c r="V28" s="6"/>
     </row>
     <row r="29" spans="1:22">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="7" t="s">
         <v>104</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -2693,7 +2702,7 @@
       <c r="V29" s="6"/>
     </row>
     <row r="30" spans="1:22">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="7" t="s">
         <v>107</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -2733,7 +2742,7 @@
       <c r="V30" s="6"/>
     </row>
     <row r="31" spans="1:22">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="7" t="s">
         <v>109</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -2773,7 +2782,7 @@
       <c r="V31" s="6"/>
     </row>
     <row r="32" spans="1:22">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="7" t="s">
         <v>112</v>
       </c>
       <c r="B32" s="3" t="s">
@@ -2813,7 +2822,7 @@
       <c r="V32" s="6"/>
     </row>
     <row r="33" spans="1:22">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="7" t="s">
         <v>115</v>
       </c>
       <c r="B33" s="3" t="s">
@@ -2853,7 +2862,7 @@
       <c r="V33" s="6"/>
     </row>
     <row r="34" spans="1:22">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="7" t="s">
         <v>118</v>
       </c>
       <c r="B34" s="3" t="s">
@@ -2893,7 +2902,7 @@
       <c r="V34" s="6"/>
     </row>
     <row r="35" spans="1:22">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="7" t="s">
         <v>119</v>
       </c>
       <c r="B35" s="3" t="s">
@@ -2933,7 +2942,7 @@
       <c r="V35" s="6"/>
     </row>
     <row r="36" spans="1:22">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="7" t="s">
         <v>123</v>
       </c>
       <c r="B36" s="3" t="s">
@@ -2973,7 +2982,7 @@
       <c r="V36" s="6"/>
     </row>
     <row r="37" spans="1:22">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="7" t="s">
         <v>127</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -3015,7 +3024,7 @@
       <c r="V37" s="6"/>
     </row>
     <row r="38" spans="1:22">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="7" t="s">
         <v>130</v>
       </c>
       <c r="B38" s="3" t="s">
@@ -3057,7 +3066,7 @@
       <c r="V38" s="6"/>
     </row>
     <row r="39" spans="1:22">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="7" t="s">
         <v>133</v>
       </c>
       <c r="B39" s="3" t="s">
@@ -3099,7 +3108,7 @@
       <c r="V39" s="6"/>
     </row>
     <row r="40" spans="1:22">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="7" t="s">
         <v>136</v>
       </c>
       <c r="B40" s="3" t="s">
@@ -3141,7 +3150,7 @@
       <c r="V40" s="6"/>
     </row>
     <row r="41" spans="1:22">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="7" t="s">
         <v>139</v>
       </c>
       <c r="B41" s="3" t="s">
@@ -3181,7 +3190,7 @@
       <c r="V41" s="6"/>
     </row>
     <row r="42" spans="1:22">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="7" t="s">
         <v>143</v>
       </c>
       <c r="B42" s="3" t="s">
@@ -3221,7 +3230,7 @@
       <c r="V42" s="6"/>
     </row>
     <row r="43" spans="1:22">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="7" t="s">
         <v>143</v>
       </c>
       <c r="B43" s="3" t="s">
@@ -3261,7 +3270,7 @@
       <c r="V43" s="6"/>
     </row>
     <row r="44" spans="1:22">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="7" t="s">
         <v>148</v>
       </c>
       <c r="B44" s="3" t="s">
@@ -3301,7 +3310,7 @@
       <c r="V44" s="6"/>
     </row>
     <row r="45" spans="1:22">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="7" t="s">
         <v>148</v>
       </c>
       <c r="B45" s="3" t="s">
@@ -3343,7 +3352,7 @@
       <c r="V45" s="6"/>
     </row>
     <row r="46" spans="1:22">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="7" t="s">
         <v>152</v>
       </c>
       <c r="B46" s="3" t="s">
@@ -3385,7 +3394,7 @@
       <c r="V46" s="6"/>
     </row>
     <row r="47" spans="1:22">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="7" t="s">
         <v>154</v>
       </c>
       <c r="B47" s="3" t="s">
@@ -3427,7 +3436,7 @@
       <c r="V47" s="6"/>
     </row>
     <row r="48" spans="1:22">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="7" t="s">
         <v>157</v>
       </c>
       <c r="B48" s="3" t="s">
@@ -3467,7 +3476,7 @@
       <c r="V48" s="6"/>
     </row>
     <row r="49" spans="1:22">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="7" t="s">
         <v>161</v>
       </c>
       <c r="B49" s="3" t="s">
@@ -3507,7 +3516,7 @@
       <c r="V49" s="6"/>
     </row>
     <row r="50" spans="1:22">
-      <c r="A50" s="3" t="s">
+      <c r="A50" s="7" t="s">
         <v>164</v>
       </c>
       <c r="B50" s="3" t="s">
@@ -3543,7 +3552,7 @@
       <c r="V50" s="6"/>
     </row>
     <row r="51" spans="1:22">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="7" t="s">
         <v>165</v>
       </c>
       <c r="B51" s="3" t="s">
@@ -3585,7 +3594,7 @@
       <c r="V51" s="6"/>
     </row>
     <row r="52" spans="1:22">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="7" t="s">
         <v>168</v>
       </c>
       <c r="B52" s="3" t="s">
@@ -3625,7 +3634,7 @@
       <c r="V52" s="6"/>
     </row>
     <row r="53" spans="1:22">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="7" t="s">
         <v>169</v>
       </c>
       <c r="B53" s="3" t="s">
@@ -3667,7 +3676,7 @@
       <c r="V53" s="6"/>
     </row>
     <row r="54" spans="1:22">
-      <c r="A54" s="3" t="s">
+      <c r="A54" s="7" t="s">
         <v>171</v>
       </c>
       <c r="B54" s="3" t="s">
@@ -3709,7 +3718,7 @@
       <c r="V54" s="6"/>
     </row>
     <row r="55" spans="1:22">
-      <c r="A55" s="3" t="s">
+      <c r="A55" s="7" t="s">
         <v>172</v>
       </c>
       <c r="B55" s="3" t="s">
@@ -3751,7 +3760,7 @@
       <c r="V55" s="6"/>
     </row>
     <row r="56" spans="1:22">
-      <c r="A56" s="3" t="s">
+      <c r="A56" s="7" t="s">
         <v>173</v>
       </c>
       <c r="B56" s="3" t="s">
@@ -3793,7 +3802,7 @@
       <c r="V56" s="6"/>
     </row>
     <row r="57" spans="1:22">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="7" t="s">
         <v>174</v>
       </c>
       <c r="B57" s="3" t="s">
@@ -3835,7 +3844,7 @@
       <c r="V57" s="6"/>
     </row>
     <row r="58" spans="1:22">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="7" t="s">
         <v>175</v>
       </c>
       <c r="B58" s="3" t="s">
@@ -3877,7 +3886,7 @@
       <c r="V58" s="6"/>
     </row>
     <row r="59" spans="1:22">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="7" t="s">
         <v>176</v>
       </c>
       <c r="B59" s="3" t="s">
@@ -3917,7 +3926,7 @@
       <c r="V59" s="6"/>
     </row>
     <row r="60" spans="1:22">
-      <c r="A60" s="3" t="s">
+      <c r="A60" s="7" t="s">
         <v>177</v>
       </c>
       <c r="B60" s="3" t="s">
@@ -3957,7 +3966,7 @@
       <c r="V60" s="6"/>
     </row>
     <row r="61" spans="1:22">
-      <c r="A61" s="3" t="s">
+      <c r="A61" s="7" t="s">
         <v>181</v>
       </c>
       <c r="B61" s="3" t="s">
@@ -3997,7 +4006,7 @@
       <c r="V61" s="6"/>
     </row>
     <row r="62" spans="1:22">
-      <c r="A62" s="3" t="s">
+      <c r="A62" s="7" t="s">
         <v>184</v>
       </c>
       <c r="B62" s="3" t="s">
@@ -4039,7 +4048,7 @@
       <c r="V62" s="6"/>
     </row>
     <row r="63" spans="1:22">
-      <c r="A63" s="3" t="s">
+      <c r="A63" s="7" t="s">
         <v>187</v>
       </c>
       <c r="B63" s="3" t="s">
@@ -4079,7 +4088,7 @@
       <c r="V63" s="6"/>
     </row>
     <row r="64" spans="1:22">
-      <c r="A64" s="3" t="s">
+      <c r="A64" s="7" t="s">
         <v>190</v>
       </c>
       <c r="B64" s="3" t="s">
@@ -4121,7 +4130,7 @@
       <c r="V64" s="6"/>
     </row>
     <row r="65" spans="1:22">
-      <c r="A65" s="3" t="s">
+      <c r="A65" s="7" t="s">
         <v>193</v>
       </c>
       <c r="B65" s="3" t="s">
@@ -4163,7 +4172,7 @@
       <c r="V65" s="6"/>
     </row>
     <row r="66" spans="1:22">
-      <c r="A66" s="3" t="s">
+      <c r="A66" s="7" t="s">
         <v>194</v>
       </c>
       <c r="B66" s="3" t="s">
@@ -4205,7 +4214,7 @@
       <c r="V66" s="6"/>
     </row>
     <row r="67" spans="1:22">
-      <c r="A67" s="3" t="s">
+      <c r="A67" s="7" t="s">
         <v>195</v>
       </c>
       <c r="B67" s="3" t="s">
@@ -4245,7 +4254,7 @@
       <c r="V67" s="6"/>
     </row>
     <row r="68" spans="1:22">
-      <c r="A68" s="3" t="s">
+      <c r="A68" s="7" t="s">
         <v>196</v>
       </c>
       <c r="B68" s="3" t="s">
@@ -4287,7 +4296,7 @@
       <c r="V68" s="6"/>
     </row>
     <row r="69" spans="1:22">
-      <c r="A69" s="3" t="s">
+      <c r="A69" s="7" t="s">
         <v>199</v>
       </c>
       <c r="B69" s="3" t="s">
@@ -4327,7 +4336,7 @@
       <c r="V69" s="6"/>
     </row>
     <row r="70" spans="1:22">
-      <c r="A70" s="3" t="s">
+      <c r="A70" s="7" t="s">
         <v>202</v>
       </c>
       <c r="B70" s="3" t="s">
@@ -4367,7 +4376,7 @@
       <c r="V70" s="6"/>
     </row>
     <row r="71" spans="1:22">
-      <c r="A71" s="3" t="s">
+      <c r="A71" s="7" t="s">
         <v>205</v>
       </c>
       <c r="B71" s="3" t="s">
@@ -4407,7 +4416,7 @@
       <c r="V71" s="6"/>
     </row>
     <row r="72" spans="1:22">
-      <c r="A72" s="3" t="s">
+      <c r="A72" s="7" t="s">
         <v>209</v>
       </c>
       <c r="B72" s="3" t="s">
@@ -4451,7 +4460,7 @@
       <c r="V72" s="6"/>
     </row>
     <row r="73" spans="1:22">
-      <c r="A73" s="3" t="s">
+      <c r="A73" s="7" t="s">
         <v>212</v>
       </c>
       <c r="B73" s="3" t="s">
@@ -4493,7 +4502,7 @@
       <c r="V73" s="6"/>
     </row>
     <row r="74" spans="1:22">
-      <c r="A74" s="3" t="s">
+      <c r="A74" s="7" t="s">
         <v>213</v>
       </c>
       <c r="B74" s="3" t="s">
@@ -4533,7 +4542,7 @@
       <c r="V74" s="6"/>
     </row>
     <row r="75" spans="1:22">
-      <c r="A75" s="3" t="s">
+      <c r="A75" s="7" t="s">
         <v>216</v>
       </c>
       <c r="B75" s="3" t="s">
@@ -4573,7 +4582,7 @@
       <c r="V75" s="6"/>
     </row>
     <row r="76" spans="1:22">
-      <c r="A76" s="3" t="s">
+      <c r="A76" s="7" t="s">
         <v>219</v>
       </c>
       <c r="B76" s="3" t="s">
@@ -4633,7 +4642,7 @@
       <c r="V76" s="6"/>
     </row>
     <row r="77" spans="1:22">
-      <c r="A77" s="3" t="s">
+      <c r="A77" s="7" t="s">
         <v>224</v>
       </c>
       <c r="B77" s="3" t="s">
@@ -4673,7 +4682,7 @@
       <c r="V77" s="6"/>
     </row>
     <row r="78" spans="1:22">
-      <c r="A78" s="3" t="s">
+      <c r="A78" s="7" t="s">
         <v>224</v>
       </c>
       <c r="B78" s="3" t="s">
@@ -4713,7 +4722,7 @@
       <c r="V78" s="6"/>
     </row>
     <row r="79" spans="1:22">
-      <c r="A79" s="3" t="s">
+      <c r="A79" s="7" t="s">
         <v>227</v>
       </c>
       <c r="B79" s="3" t="s">
@@ -4755,7 +4764,7 @@
       <c r="V79" s="6"/>
     </row>
     <row r="80" spans="1:22">
-      <c r="A80" s="3" t="s">
+      <c r="A80" s="7" t="s">
         <v>227</v>
       </c>
       <c r="B80" s="3" t="s">
@@ -4795,7 +4804,7 @@
       <c r="V80" s="6"/>
     </row>
     <row r="81" spans="1:22">
-      <c r="A81" s="3" t="s">
+      <c r="A81" s="7" t="s">
         <v>231</v>
       </c>
       <c r="B81" s="3" t="s">
@@ -4835,7 +4844,7 @@
       <c r="V81" s="6"/>
     </row>
     <row r="82" spans="1:22">
-      <c r="A82" s="3" t="s">
+      <c r="A82" s="7" t="s">
         <v>233</v>
       </c>
       <c r="B82" s="3" t="s">
@@ -4877,7 +4886,7 @@
       <c r="V82" s="6"/>
     </row>
     <row r="83" spans="1:22">
-      <c r="A83" s="3" t="s">
+      <c r="A83" s="7" t="s">
         <v>237</v>
       </c>
       <c r="B83" s="3" t="s">
@@ -4919,7 +4928,7 @@
       <c r="V83" s="6"/>
     </row>
     <row r="84" spans="1:22">
-      <c r="A84" s="3" t="s">
+      <c r="A84" s="7" t="s">
         <v>237</v>
       </c>
       <c r="B84" s="3" t="s">
@@ -4961,7 +4970,7 @@
       <c r="V84" s="6"/>
     </row>
     <row r="85" spans="1:22">
-      <c r="A85" s="3" t="s">
+      <c r="A85" s="7" t="s">
         <v>242</v>
       </c>
       <c r="B85" s="3" t="s">
@@ -5001,7 +5010,7 @@
       <c r="V85" s="6"/>
     </row>
     <row r="86" spans="1:22">
-      <c r="A86" s="3" t="s">
+      <c r="A86" s="7" t="s">
         <v>244</v>
       </c>
       <c r="B86" s="3" t="s">
@@ -5041,7 +5050,7 @@
       <c r="V86" s="6"/>
     </row>
     <row r="87" spans="1:22">
-      <c r="A87" s="3" t="s">
+      <c r="A87" s="7" t="s">
         <v>248</v>
       </c>
       <c r="B87" s="3" t="s">
@@ -5081,7 +5090,7 @@
       <c r="V87" s="6"/>
     </row>
     <row r="88" spans="1:22">
-      <c r="A88" s="3" t="s">
+      <c r="A88" s="7" t="s">
         <v>252</v>
       </c>
       <c r="B88" s="3" t="s">
@@ -5121,7 +5130,7 @@
       <c r="V88" s="6"/>
     </row>
     <row r="89" spans="1:22">
-      <c r="A89" s="3" t="s">
+      <c r="A89" s="7" t="s">
         <v>255</v>
       </c>
       <c r="B89" s="3" t="s">
@@ -5161,7 +5170,7 @@
       <c r="V89" s="6"/>
     </row>
     <row r="90" spans="1:22">
-      <c r="A90" s="3" t="s">
+      <c r="A90" s="7" t="s">
         <v>257</v>
       </c>
       <c r="B90" s="3" t="s">
@@ -5203,7 +5212,7 @@
       <c r="V90" s="6"/>
     </row>
     <row r="91" spans="1:22">
-      <c r="A91" s="3" t="s">
+      <c r="A91" s="7" t="s">
         <v>259</v>
       </c>
       <c r="B91" s="3" t="s">
@@ -5245,7 +5254,7 @@
       <c r="V91" s="6"/>
     </row>
     <row r="92" spans="1:22">
-      <c r="A92" s="3" t="s">
+      <c r="A92" s="7" t="s">
         <v>261</v>
       </c>
       <c r="B92" s="3" t="s">
@@ -5285,7 +5294,7 @@
       <c r="V92" s="6"/>
     </row>
     <row r="93" spans="1:22">
-      <c r="A93" s="3" t="s">
+      <c r="A93" s="7" t="s">
         <v>263</v>
       </c>
       <c r="B93" s="3" t="s">
@@ -5327,7 +5336,7 @@
       <c r="V93" s="6"/>
     </row>
     <row r="94" spans="1:22">
-      <c r="A94" s="3" t="s">
+      <c r="A94" s="7" t="s">
         <v>267</v>
       </c>
       <c r="B94" s="3" t="s">
@@ -5369,7 +5378,7 @@
       <c r="V94" s="6"/>
     </row>
     <row r="95" spans="1:22">
-      <c r="A95" s="3" t="s">
+      <c r="A95" s="7" t="s">
         <v>271</v>
       </c>
       <c r="B95" s="3" t="s">
@@ -5411,7 +5420,7 @@
       <c r="V95" s="6"/>
     </row>
     <row r="96" spans="1:22">
-      <c r="A96" s="3" t="s">
+      <c r="A96" s="7" t="s">
         <v>272</v>
       </c>
       <c r="B96" s="3" t="s">
@@ -5451,7 +5460,7 @@
       <c r="V96" s="6"/>
     </row>
     <row r="97" spans="1:22">
-      <c r="A97" s="3" t="s">
+      <c r="A97" s="7" t="s">
         <v>274</v>
       </c>
       <c r="B97" s="3" t="s">
@@ -5493,7 +5502,7 @@
       <c r="V97" s="6"/>
     </row>
     <row r="98" spans="1:22">
-      <c r="A98" s="3" t="s">
+      <c r="A98" s="7" t="s">
         <v>274</v>
       </c>
       <c r="B98" s="3" t="s">
@@ -5533,7 +5542,7 @@
       <c r="V98" s="6"/>
     </row>
     <row r="99" spans="1:22">
-      <c r="A99" s="3" t="s">
+      <c r="A99" s="7" t="s">
         <v>277</v>
       </c>
       <c r="B99" s="3" t="s">
@@ -5575,7 +5584,7 @@
       <c r="V99" s="6"/>
     </row>
     <row r="100" spans="1:22">
-      <c r="A100" s="3" t="s">
+      <c r="A100" s="7" t="s">
         <v>278</v>
       </c>
       <c r="B100" s="3" t="s">
@@ -5617,7 +5626,7 @@
       <c r="V100" s="6"/>
     </row>
     <row r="101" spans="1:22">
-      <c r="A101" s="3" t="s">
+      <c r="A101" s="7" t="s">
         <v>281</v>
       </c>
       <c r="B101" s="3" t="s">
@@ -5659,7 +5668,7 @@
       <c r="V101" s="6"/>
     </row>
     <row r="102" spans="1:22">
-      <c r="A102" s="3" t="s">
+      <c r="A102" s="7" t="s">
         <v>283</v>
       </c>
       <c r="B102" s="3" t="s">
@@ -5699,7 +5708,7 @@
       <c r="V102" s="6"/>
     </row>
     <row r="103" spans="1:22">
-      <c r="A103" s="3" t="s">
+      <c r="A103" s="7" t="s">
         <v>286</v>
       </c>
       <c r="B103" s="3" t="s">
@@ -5739,7 +5748,7 @@
       <c r="V103" s="6"/>
     </row>
     <row r="104" spans="1:22">
-      <c r="A104" s="3" t="s">
+      <c r="A104" s="7" t="s">
         <v>290</v>
       </c>
       <c r="B104" s="3" t="s">
@@ -5779,7 +5788,7 @@
       <c r="V104" s="6"/>
     </row>
     <row r="105" spans="1:22">
-      <c r="A105" s="3" t="s">
+      <c r="A105" s="7" t="s">
         <v>291</v>
       </c>
       <c r="B105" s="3" t="s">
@@ -5819,7 +5828,7 @@
       <c r="V105" s="6"/>
     </row>
     <row r="106" spans="1:22">
-      <c r="A106" s="3" t="s">
+      <c r="A106" s="7" t="s">
         <v>292</v>
       </c>
       <c r="B106" s="3" t="s">
@@ -5859,7 +5868,7 @@
       <c r="V106" s="6"/>
     </row>
     <row r="107" spans="1:22">
-      <c r="A107" s="3" t="s">
+      <c r="A107" s="7" t="s">
         <v>293</v>
       </c>
       <c r="B107" s="3" t="s">
@@ -5899,7 +5908,7 @@
       <c r="V107" s="6"/>
     </row>
     <row r="108" spans="1:22">
-      <c r="A108" s="3" t="s">
+      <c r="A108" s="7" t="s">
         <v>294</v>
       </c>
       <c r="B108" s="3" t="s">
@@ -5939,7 +5948,7 @@
       <c r="V108" s="6"/>
     </row>
     <row r="109" spans="1:22">
-      <c r="A109" s="3" t="s">
+      <c r="A109" s="7" t="s">
         <v>296</v>
       </c>
       <c r="B109" s="3" t="s">
@@ -5979,7 +5988,7 @@
       <c r="V109" s="6"/>
     </row>
     <row r="110" spans="1:22">
-      <c r="A110" s="3" t="s">
+      <c r="A110" s="7" t="s">
         <v>299</v>
       </c>
       <c r="B110" s="3" t="s">
@@ -6021,7 +6030,7 @@
       <c r="V110" s="6"/>
     </row>
     <row r="111" spans="1:22">
-      <c r="A111" s="3" t="s">
+      <c r="A111" s="7" t="s">
         <v>300</v>
       </c>
       <c r="B111" s="3" t="s">
@@ -6061,7 +6070,7 @@
       <c r="V111" s="6"/>
     </row>
     <row r="112" spans="1:22">
-      <c r="A112" s="3" t="s">
+      <c r="A112" s="7" t="s">
         <v>300</v>
       </c>
       <c r="B112" s="3" t="s">
@@ -6103,7 +6112,7 @@
       <c r="V112" s="6"/>
     </row>
     <row r="113" spans="1:22">
-      <c r="A113" s="3" t="s">
+      <c r="A113" s="7" t="s">
         <v>303</v>
       </c>
       <c r="B113" s="3" t="s">
@@ -6143,7 +6152,7 @@
       <c r="V113" s="6"/>
     </row>
     <row r="114" spans="1:22">
-      <c r="A114" s="3" t="s">
+      <c r="A114" s="7" t="s">
         <v>305</v>
       </c>
       <c r="B114" s="3" t="s">
@@ -6152,8 +6161,12 @@
       <c r="C114" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="D114" s="3"/>
-      <c r="E114" s="3"/>
+      <c r="D114" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="E114" s="3" t="s">
+        <v>307</v>
+      </c>
       <c r="F114" s="3">
         <v>80</v>
       </c>
@@ -6179,8 +6192,8 @@
       <c r="V114" s="6"/>
     </row>
     <row r="115" spans="1:22">
-      <c r="A115" s="3" t="s">
-        <v>306</v>
+      <c r="A115" s="7" t="s">
+        <v>308</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>273</v>
@@ -6219,8 +6232,8 @@
       <c r="V115" s="6"/>
     </row>
     <row r="116" spans="1:22">
-      <c r="A116" s="3" t="s">
-        <v>306</v>
+      <c r="A116" s="7" t="s">
+        <v>308</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>158</v>
@@ -6259,8 +6272,8 @@
       <c r="V116" s="6"/>
     </row>
     <row r="117" spans="1:22">
-      <c r="A117" s="3" t="s">
-        <v>307</v>
+      <c r="A117" s="7" t="s">
+        <v>309</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>97</v>
@@ -6299,14 +6312,14 @@
       <c r="V117" s="6"/>
     </row>
     <row r="118" spans="1:22">
-      <c r="A118" s="3" t="s">
-        <v>307</v>
+      <c r="A118" s="7" t="s">
+        <v>309</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="D118" s="3" t="s">
         <v>59</v>
@@ -6341,8 +6354,8 @@
       <c r="V118" s="6"/>
     </row>
     <row r="119" spans="1:22">
-      <c r="A119" s="3" t="s">
-        <v>307</v>
+      <c r="A119" s="7" t="s">
+        <v>309</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>33</v>
@@ -6381,8 +6394,8 @@
       <c r="V119" s="6"/>
     </row>
     <row r="120" spans="1:22">
-      <c r="A120" s="3" t="s">
-        <v>309</v>
+      <c r="A120" s="7" t="s">
+        <v>311</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>58</v>
@@ -6391,10 +6404,10 @@
         <v>3</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="F120" s="3">
         <v>75</v>
@@ -6421,8 +6434,8 @@
       <c r="V120" s="6"/>
     </row>
     <row r="121" spans="1:22">
-      <c r="A121" s="3" t="s">
-        <v>312</v>
+      <c r="A121" s="7" t="s">
+        <v>314</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>19</v>
@@ -6463,8 +6476,8 @@
       <c r="V121" s="6"/>
     </row>
     <row r="122" spans="1:22">
-      <c r="A122" s="3" t="s">
-        <v>313</v>
+      <c r="A122" s="7" t="s">
+        <v>315</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>29</v>
@@ -6505,8 +6518,8 @@
       <c r="V122" s="6"/>
     </row>
     <row r="123" spans="1:22">
-      <c r="A123" s="3" t="s">
-        <v>314</v>
+      <c r="A123" s="7" t="s">
+        <v>316</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>89</v>
@@ -6547,8 +6560,8 @@
       <c r="V123" s="6"/>
     </row>
     <row r="124" spans="1:22">
-      <c r="A124" s="3" t="s">
-        <v>315</v>
+      <c r="A124" s="7" t="s">
+        <v>317</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>89</v>
@@ -6557,10 +6570,10 @@
         <v>163</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="F124" s="3">
         <v>72</v>
@@ -6589,8 +6602,8 @@
       <c r="V124" s="6"/>
     </row>
     <row r="125" spans="1:22">
-      <c r="A125" s="3" t="s">
-        <v>318</v>
+      <c r="A125" s="7" t="s">
+        <v>320</v>
       </c>
       <c r="B125" s="3" t="s">
         <v>89</v>
@@ -6599,10 +6612,10 @@
         <v>163</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="F125" s="3">
         <v>72</v>
@@ -6631,8 +6644,8 @@
       <c r="V125" s="6"/>
     </row>
     <row r="126" spans="1:22">
-      <c r="A126" s="3" t="s">
-        <v>321</v>
+      <c r="A126" s="7" t="s">
+        <v>323</v>
       </c>
       <c r="B126" s="3" t="s">
         <v>273</v>
@@ -6667,8 +6680,8 @@
       <c r="V126" s="6"/>
     </row>
     <row r="127" spans="1:22">
-      <c r="A127" s="3" t="s">
-        <v>322</v>
+      <c r="A127" s="7" t="s">
+        <v>324</v>
       </c>
       <c r="B127" s="3" t="s">
         <v>83</v>
@@ -6709,8 +6722,8 @@
       <c r="V127" s="6"/>
     </row>
     <row r="128" spans="1:22">
-      <c r="A128" s="3" t="s">
-        <v>323</v>
+      <c r="A128" s="7" t="s">
+        <v>325</v>
       </c>
       <c r="B128" s="3" t="s">
         <v>83</v>
@@ -6751,8 +6764,8 @@
       <c r="V128" s="6"/>
     </row>
     <row r="129" spans="1:22">
-      <c r="A129" s="3" t="s">
-        <v>324</v>
+      <c r="A129" s="7" t="s">
+        <v>326</v>
       </c>
       <c r="B129" s="3" t="s">
         <v>158</v>
@@ -6761,10 +6774,10 @@
         <v>3</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="F129" s="3">
         <v>75</v>
@@ -6791,8 +6804,8 @@
       <c r="V129" s="6"/>
     </row>
     <row r="130" spans="1:22">
-      <c r="A130" s="3" t="s">
-        <v>327</v>
+      <c r="A130" s="7" t="s">
+        <v>329</v>
       </c>
       <c r="B130" s="3" t="s">
         <v>83</v>
@@ -6833,8 +6846,8 @@
       <c r="V130" s="6"/>
     </row>
     <row r="131" spans="1:22">
-      <c r="A131" s="3" t="s">
-        <v>328</v>
+      <c r="A131" s="7" t="s">
+        <v>330</v>
       </c>
       <c r="B131" s="3" t="s">
         <v>97</v>
@@ -6873,8 +6886,8 @@
       <c r="V131" s="6"/>
     </row>
     <row r="132" spans="1:22">
-      <c r="A132" s="3" t="s">
-        <v>329</v>
+      <c r="A132" s="7" t="s">
+        <v>331</v>
       </c>
       <c r="B132" s="3" t="s">
         <v>97</v>
@@ -6883,10 +6896,10 @@
         <v>3</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="F132" s="3">
         <v>75</v>
@@ -6913,8 +6926,8 @@
       <c r="V132" s="6"/>
     </row>
     <row r="133" spans="1:22">
-      <c r="A133" s="3" t="s">
-        <v>332</v>
+      <c r="A133" s="7" t="s">
+        <v>334</v>
       </c>
       <c r="B133" s="3" t="s">
         <v>158</v>
@@ -6953,20 +6966,20 @@
       <c r="V133" s="6"/>
     </row>
     <row r="134" spans="1:22">
-      <c r="A134" s="3" t="s">
-        <v>333</v>
+      <c r="A134" s="7" t="s">
+        <v>335</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="F134" s="3"/>
       <c r="G134" s="3">
@@ -6993,8 +7006,8 @@
       <c r="V134" s="6"/>
     </row>
     <row r="135" spans="1:22">
-      <c r="A135" s="3" t="s">
-        <v>337</v>
+      <c r="A135" s="7" t="s">
+        <v>339</v>
       </c>
       <c r="B135" s="3" t="s">
         <v>83</v>
@@ -7035,8 +7048,8 @@
       <c r="V135" s="6"/>
     </row>
     <row r="136" spans="1:22">
-      <c r="A136" s="3" t="s">
-        <v>338</v>
+      <c r="A136" s="7" t="s">
+        <v>340</v>
       </c>
       <c r="B136" s="3" t="s">
         <v>97</v>
@@ -7075,8 +7088,8 @@
       <c r="V136" s="6"/>
     </row>
     <row r="137" spans="1:22">
-      <c r="A137" s="3" t="s">
-        <v>339</v>
+      <c r="A137" s="7" t="s">
+        <v>341</v>
       </c>
       <c r="B137" s="3" t="s">
         <v>97</v>
@@ -7115,8 +7128,8 @@
       <c r="V137" s="6"/>
     </row>
     <row r="138" spans="1:22">
-      <c r="A138" s="3" t="s">
-        <v>340</v>
+      <c r="A138" s="7" t="s">
+        <v>342</v>
       </c>
       <c r="B138" s="3" t="s">
         <v>178</v>
@@ -7155,8 +7168,8 @@
       <c r="V138" s="6"/>
     </row>
     <row r="139" spans="1:22">
-      <c r="A139" s="3" t="s">
-        <v>341</v>
+      <c r="A139" s="7" t="s">
+        <v>343</v>
       </c>
       <c r="B139" s="3" t="s">
         <v>178</v>
@@ -7195,8 +7208,8 @@
       <c r="V139" s="6"/>
     </row>
     <row r="140" spans="1:22">
-      <c r="A140" s="3" t="s">
-        <v>342</v>
+      <c r="A140" s="7" t="s">
+        <v>344</v>
       </c>
       <c r="B140" s="3" t="s">
         <v>273</v>
@@ -7235,8 +7248,8 @@
       <c r="V140" s="6"/>
     </row>
     <row r="141" spans="1:22">
-      <c r="A141" s="3" t="s">
-        <v>343</v>
+      <c r="A141" s="7" t="s">
+        <v>345</v>
       </c>
       <c r="B141" s="3" t="s">
         <v>63</v>
@@ -7275,8 +7288,8 @@
       <c r="V141" s="6"/>
     </row>
     <row r="142" spans="1:22">
-      <c r="A142" s="3" t="s">
-        <v>344</v>
+      <c r="A142" s="7" t="s">
+        <v>346</v>
       </c>
       <c r="B142" s="3" t="s">
         <v>58</v>
@@ -7315,8 +7328,8 @@
       <c r="V142" s="6"/>
     </row>
     <row r="143" spans="1:22">
-      <c r="A143" s="3" t="s">
-        <v>345</v>
+      <c r="A143" s="7" t="s">
+        <v>347</v>
       </c>
       <c r="B143" s="3" t="s">
         <v>58</v>
@@ -7351,8 +7364,8 @@
       <c r="V143" s="6"/>
     </row>
     <row r="144" spans="1:22">
-      <c r="A144" s="3" t="s">
-        <v>346</v>
+      <c r="A144" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="B144" s="3" t="s">
         <v>273</v>
@@ -7391,8 +7404,8 @@
       <c r="V144" s="6"/>
     </row>
     <row r="145" spans="1:22">
-      <c r="A145" s="3" t="s">
-        <v>347</v>
+      <c r="A145" s="7" t="s">
+        <v>349</v>
       </c>
       <c r="B145" s="3" t="s">
         <v>33</v>
@@ -7433,8 +7446,8 @@
       <c r="V145" s="6"/>
     </row>
     <row r="146" spans="1:22">
-      <c r="A146" s="3" t="s">
-        <v>348</v>
+      <c r="A146" s="7" t="s">
+        <v>350</v>
       </c>
       <c r="B146" s="3" t="s">
         <v>19</v>
@@ -7475,8 +7488,8 @@
       <c r="V146" s="6"/>
     </row>
     <row r="147" spans="1:22">
-      <c r="A147" s="3" t="s">
-        <v>349</v>
+      <c r="A147" s="7" t="s">
+        <v>351</v>
       </c>
       <c r="B147" s="3" t="s">
         <v>68</v>
@@ -7485,10 +7498,10 @@
         <v>163</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F147" s="3">
         <v>67.5</v>
@@ -7515,14 +7528,14 @@
       <c r="V147" s="6"/>
     </row>
     <row r="148" spans="1:22">
-      <c r="A148" s="3" t="s">
-        <v>352</v>
+      <c r="A148" s="7" t="s">
+        <v>354</v>
       </c>
       <c r="B148" s="3" t="s">
         <v>124</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="D148" s="3" t="s">
         <v>235</v>
@@ -7553,30 +7566,6 @@
       <c r="T148" s="5"/>
       <c r="U148" s="6"/>
       <c r="V148" s="6"/>
-    </row>
-    <row r="149" spans="1:22">
-      <c r="A149" s="3"/>
-      <c r="B149" s="3"/>
-      <c r="C149" s="3"/>
-      <c r="D149" s="3"/>
-      <c r="E149" s="3"/>
-      <c r="F149" s="3"/>
-      <c r="G149" s="3"/>
-      <c r="H149" s="3"/>
-      <c r="I149" s="3"/>
-      <c r="J149" s="3"/>
-      <c r="K149" s="5"/>
-      <c r="L149" s="5"/>
-      <c r="M149" s="6"/>
-      <c r="N149" s="6"/>
-      <c r="O149" s="5"/>
-      <c r="P149" s="5"/>
-      <c r="Q149" s="6"/>
-      <c r="R149" s="6"/>
-      <c r="S149" s="5"/>
-      <c r="T149" s="5"/>
-      <c r="U149" s="6"/>
-      <c r="V149" s="6"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>